<commit_message>
Added Funtion to get data from excell
</commit_message>
<xml_diff>
--- a/ExcelData/wizcomDemoAccount.xlsx
+++ b/ExcelData/wizcomDemoAccount.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
   <si>
     <t>demo@sourcewiz.co</t>
   </si>
@@ -20,7 +20,25 @@
     <t/>
   </si>
   <si>
+    <t>Searching Data</t>
+  </si>
+  <si>
+    <t>Customer_Search</t>
+  </si>
+  <si>
+    <t>Account_Name</t>
+  </si>
+  <si>
     <t>xyz@sourcewiz.co</t>
+  </si>
+  <si>
+    <t>sofa</t>
+  </si>
+  <si>
+    <t>Heman Test</t>
+  </si>
+  <si>
+    <t>DC</t>
   </si>
   <si>
     <t>admin123</t>
@@ -29,20 +47,17 @@
     <t>lui</t>
   </si>
   <si>
-    <t>qateam@wizcommerce.com</t>
+    <t>tech@wizcommerce.com</t>
   </si>
   <si>
     <t>admin</t>
-  </si>
-  <si>
-    <t>tech@wizcommerce.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -64,6 +79,11 @@
       <sz val="11.0"/>
       <color theme="10"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -95,21 +115,22 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf quotePrefix="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf quotePrefix="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf quotePrefix="1" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -331,7 +352,11 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="18.29"/>
-    <col customWidth="1" min="2" max="6" width="8.71"/>
+    <col customWidth="1" min="2" max="2" width="8.71"/>
+    <col customWidth="1" min="3" max="3" width="16.14"/>
+    <col customWidth="1" min="4" max="4" width="21.86"/>
+    <col customWidth="1" min="5" max="5" width="15.71"/>
+    <col customWidth="1" min="6" max="6" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -341,37 +366,55 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="3" t="s">
-        <v>2</v>
+      <c r="A2" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="C2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>3</v>
+      <c r="B3" s="7" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="3" t="s">
-        <v>2</v>
+      <c r="A4" s="4" t="s">
+        <v>5</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>4</v>
+      <c r="B4" s="7" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1"/>
@@ -1392,27 +1435,27 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="5" t="s">
-        <v>5</v>
+      <c r="A2" s="4" t="s">
+        <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>6</v>
+      <c r="B2" s="7" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="3" t="s">
-        <v>7</v>
+      <c r="A3" s="4" t="s">
+        <v>11</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>6</v>
+      <c r="B3" s="7" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1"/>
@@ -2415,11 +2458,12 @@
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="A1"/>
-    <hyperlink r:id="rId2" ref="A3"/>
+    <hyperlink r:id="rId2" ref="A2"/>
+    <hyperlink r:id="rId3" ref="A3"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait"/>
-  <drawing r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>